<commit_message>
Small improvements and typos.
</commit_message>
<xml_diff>
--- a/biological studies.xlsx
+++ b/biological studies.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tobiaochsner/Documents/Thesis/branch-lengths-paper/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{A3E430FB-1D5C-214A-A383-B0C7081DCEF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B077052-061F-5F4B-9D53-1140A5AB1A4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="18380" xr2:uid="{B5FD0977-0991-D648-A373-806D6CB44D67}"/>
   </bookViews>
@@ -3581,8 +3581,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C32FE525-9392-C64B-BB12-6C5F047EE504}">
   <dimension ref="A1:J259"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="B183" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I209" sqref="I209"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9142,7 +9142,7 @@
       <c r="G208" t="s">
         <v>799</v>
       </c>
-      <c r="H208" t="s">
+      <c r="I208" t="s">
         <v>840</v>
       </c>
       <c r="J208" t="s">
@@ -9171,7 +9171,7 @@
       <c r="G209" t="s">
         <v>799</v>
       </c>
-      <c r="H209" t="s">
+      <c r="I209" t="s">
         <v>840</v>
       </c>
       <c r="J209" t="s">
@@ -9200,7 +9200,7 @@
       <c r="G210" t="s">
         <v>799</v>
       </c>
-      <c r="H210" t="s">
+      <c r="I210" t="s">
         <v>841</v>
       </c>
       <c r="J210" t="s">

</xml_diff>